<commit_message>
first complete draft of dataset
</commit_message>
<xml_diff>
--- a/virginiaSuicideDataSet.xlsx
+++ b/virginiaSuicideDataSet.xlsx
@@ -453,18 +453,12 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -479,10 +473,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,9 +808,9 @@
   <dimension ref="A2:H572"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1300" topLeftCell="A382" activePane="bottomLeft"/>
+      <pane ySplit="1300" topLeftCell="A526" activePane="bottomLeft"/>
       <selection activeCell="G2" sqref="G2"/>
-      <selection pane="bottomLeft" activeCell="H380" sqref="H380"/>
+      <selection pane="bottomLeft" activeCell="H381" sqref="H381"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1005,6 +998,9 @@
       <c r="G8">
         <v>1357</v>
       </c>
+      <c r="H8">
+        <v>93</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -1158,6 +1154,9 @@
       <c r="G14">
         <v>2874</v>
       </c>
+      <c r="H14">
+        <v>211</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
@@ -1311,6 +1310,9 @@
       <c r="G20">
         <v>616</v>
       </c>
+      <c r="H20">
+        <v>66</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
@@ -1464,6 +1466,9 @@
       <c r="G26">
         <v>465</v>
       </c>
+      <c r="H26">
+        <v>54</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
@@ -1617,6 +1622,9 @@
       <c r="G32">
         <v>1139</v>
       </c>
+      <c r="H32">
+        <v>87</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
@@ -1770,6 +1778,9 @@
       <c r="G38">
         <v>549</v>
       </c>
+      <c r="H38">
+        <v>31</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
@@ -1923,6 +1934,9 @@
       <c r="G44">
         <v>5387</v>
       </c>
+      <c r="H44">
+        <v>316</v>
+      </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
@@ -2076,6 +2090,9 @@
       <c r="G50">
         <v>2397</v>
       </c>
+      <c r="H50">
+        <v>227</v>
+      </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
@@ -2229,6 +2246,9 @@
       <c r="G56">
         <v>158</v>
       </c>
+      <c r="H56">
+        <v>13</v>
+      </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
@@ -2382,6 +2402,9 @@
       <c r="G62">
         <v>2273</v>
       </c>
+      <c r="H62">
+        <v>258</v>
+      </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
@@ -2535,6 +2558,9 @@
       <c r="G68">
         <v>218</v>
       </c>
+      <c r="H68">
+        <v>35</v>
+      </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
@@ -2688,6 +2714,9 @@
       <c r="G74">
         <v>1066</v>
       </c>
+      <c r="H74">
+        <v>120</v>
+      </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
@@ -2841,6 +2870,9 @@
       <c r="G80">
         <v>740</v>
       </c>
+      <c r="H80">
+        <v>38</v>
+      </c>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
@@ -2994,6 +3026,9 @@
       <c r="G86">
         <v>721</v>
       </c>
+      <c r="H86">
+        <v>94</v>
+      </c>
     </row>
     <row r="87" spans="1:8">
       <c r="A87" t="s">
@@ -3147,6 +3182,9 @@
       <c r="G92">
         <v>658</v>
       </c>
+      <c r="H92">
+        <v>68</v>
+      </c>
     </row>
     <row r="93" spans="1:8">
       <c r="A93" t="s">
@@ -3300,6 +3338,9 @@
       <c r="G98">
         <v>1964</v>
       </c>
+      <c r="H98">
+        <v>137</v>
+      </c>
     </row>
     <row r="99" spans="1:8">
       <c r="A99" t="s">
@@ -3453,6 +3494,9 @@
       <c r="G104">
         <v>1232</v>
       </c>
+      <c r="H104">
+        <v>58</v>
+      </c>
     </row>
     <row r="105" spans="1:8">
       <c r="A105" t="s">
@@ -3606,6 +3650,9 @@
       <c r="G110">
         <v>1340</v>
       </c>
+      <c r="H110">
+        <v>169</v>
+      </c>
     </row>
     <row r="111" spans="1:8">
       <c r="A111" t="s">
@@ -3759,6 +3806,9 @@
       <c r="G116">
         <v>335</v>
       </c>
+      <c r="H116">
+        <v>15</v>
+      </c>
     </row>
     <row r="117" spans="1:8">
       <c r="A117" t="s">
@@ -3912,6 +3962,9 @@
       <c r="G122">
         <v>521</v>
       </c>
+      <c r="H122">
+        <v>35</v>
+      </c>
     </row>
     <row r="123" spans="1:8">
       <c r="A123" t="s">
@@ -4065,6 +4118,9 @@
       <c r="G128">
         <v>11590</v>
       </c>
+      <c r="H128">
+        <v>1106</v>
+      </c>
     </row>
     <row r="129" spans="1:8">
       <c r="A129" t="s">
@@ -4218,6 +4274,9 @@
       <c r="G134">
         <v>413</v>
       </c>
+      <c r="H134">
+        <v>41</v>
+      </c>
     </row>
     <row r="135" spans="1:8">
       <c r="A135" t="s">
@@ -4371,6 +4430,9 @@
       <c r="G140">
         <v>191</v>
       </c>
+      <c r="H140">
+        <v>11</v>
+      </c>
     </row>
     <row r="141" spans="1:8">
       <c r="A141" t="s">
@@ -4524,6 +4586,9 @@
       <c r="G146">
         <v>1504</v>
       </c>
+      <c r="H146">
+        <v>131</v>
+      </c>
     </row>
     <row r="147" spans="1:8">
       <c r="A147" t="s">
@@ -4677,6 +4742,9 @@
       <c r="G152">
         <v>338</v>
       </c>
+      <c r="H152">
+        <v>34</v>
+      </c>
     </row>
     <row r="153" spans="1:8">
       <c r="A153" t="s">
@@ -4830,6 +4898,9 @@
       <c r="G158">
         <v>514</v>
       </c>
+      <c r="H158">
+        <v>62</v>
+      </c>
     </row>
     <row r="159" spans="1:8">
       <c r="A159" t="s">
@@ -4983,6 +5054,9 @@
       <c r="G164">
         <v>1059</v>
       </c>
+      <c r="H164">
+        <v>90</v>
+      </c>
     </row>
     <row r="165" spans="1:8">
       <c r="A165" t="s">
@@ -5136,6 +5210,9 @@
       <c r="G170">
         <v>467</v>
       </c>
+      <c r="H170">
+        <v>38</v>
+      </c>
     </row>
     <row r="171" spans="1:8">
       <c r="A171" t="s">
@@ -5289,6 +5366,9 @@
       <c r="G176">
         <v>28905</v>
       </c>
+      <c r="H176">
+        <v>3559</v>
+      </c>
     </row>
     <row r="177" spans="1:8">
       <c r="A177" t="s">
@@ -5442,6 +5522,9 @@
       <c r="G182">
         <v>1859</v>
       </c>
+      <c r="H182">
+        <v>183</v>
+      </c>
     </row>
     <row r="183" spans="1:8">
       <c r="A183" t="s">
@@ -5595,6 +5678,9 @@
       <c r="G188">
         <v>525</v>
       </c>
+      <c r="H188">
+        <v>50</v>
+      </c>
     </row>
     <row r="189" spans="1:8">
       <c r="A189" t="s">
@@ -5748,6 +5834,9 @@
       <c r="G194">
         <v>760</v>
       </c>
+      <c r="H194">
+        <v>54</v>
+      </c>
     </row>
     <row r="195" spans="1:8">
       <c r="A195" t="s">
@@ -5901,6 +5990,9 @@
       <c r="G200">
         <v>1936</v>
       </c>
+      <c r="H200">
+        <v>215</v>
+      </c>
     </row>
     <row r="201" spans="1:8">
       <c r="A201" t="s">
@@ -6054,6 +6146,9 @@
       <c r="G206">
         <v>2747</v>
       </c>
+      <c r="H206">
+        <v>359</v>
+      </c>
     </row>
     <row r="207" spans="1:8">
       <c r="A207" t="s">
@@ -6207,6 +6302,9 @@
       <c r="G212">
         <v>632</v>
       </c>
+      <c r="H212">
+        <v>103</v>
+      </c>
     </row>
     <row r="213" spans="1:8">
       <c r="A213" t="s">
@@ -6360,6 +6458,9 @@
       <c r="G218">
         <v>1198</v>
       </c>
+      <c r="H218">
+        <v>173</v>
+      </c>
     </row>
     <row r="219" spans="1:8">
       <c r="A219" t="s">
@@ -6513,6 +6614,9 @@
       <c r="G224">
         <v>664</v>
       </c>
+      <c r="H224">
+        <v>52</v>
+      </c>
     </row>
     <row r="225" spans="1:8">
       <c r="A225" t="s">
@@ -6666,6 +6770,9 @@
       <c r="G230">
         <v>723</v>
       </c>
+      <c r="H230">
+        <v>91</v>
+      </c>
     </row>
     <row r="231" spans="1:8">
       <c r="A231" t="s">
@@ -6819,6 +6926,9 @@
       <c r="G236">
         <v>583</v>
       </c>
+      <c r="H236">
+        <v>48</v>
+      </c>
     </row>
     <row r="237" spans="1:8">
       <c r="A237" t="s">
@@ -6972,6 +7082,9 @@
       <c r="G242">
         <v>418</v>
       </c>
+      <c r="H242">
+        <v>46</v>
+      </c>
     </row>
     <row r="243" spans="1:8">
       <c r="A243" t="s">
@@ -7125,6 +7238,9 @@
       <c r="G248">
         <v>1771</v>
       </c>
+      <c r="H248">
+        <v>136</v>
+      </c>
     </row>
     <row r="249" spans="1:8">
       <c r="A249" t="s">
@@ -7278,6 +7394,9 @@
       <c r="G254">
         <v>3322</v>
       </c>
+      <c r="H254">
+        <v>343</v>
+      </c>
     </row>
     <row r="255" spans="1:8">
       <c r="A255" t="s">
@@ -7431,6 +7550,9 @@
       <c r="G260">
         <v>11361</v>
       </c>
+      <c r="H260">
+        <v>1001</v>
+      </c>
     </row>
     <row r="261" spans="1:8">
       <c r="A261" t="s">
@@ -7584,6 +7706,9 @@
       <c r="G266">
         <v>2845</v>
       </c>
+      <c r="H266">
+        <v>206</v>
+      </c>
     </row>
     <row r="267" spans="1:8">
       <c r="A267" t="s">
@@ -7737,6 +7862,9 @@
       <c r="G272">
         <v>81</v>
       </c>
+      <c r="H272">
+        <v>5</v>
+      </c>
     </row>
     <row r="273" spans="1:8">
       <c r="A273" t="s">
@@ -7890,6 +8018,9 @@
       <c r="G278">
         <v>1286</v>
       </c>
+      <c r="H278">
+        <v>93</v>
+      </c>
     </row>
     <row r="279" spans="1:8">
       <c r="A279" t="s">
@@ -8043,6 +8174,9 @@
       <c r="G284">
         <v>2102</v>
       </c>
+      <c r="H284">
+        <v>174</v>
+      </c>
     </row>
     <row r="285" spans="1:8">
       <c r="A285" t="s">
@@ -8196,6 +8330,9 @@
       <c r="G290">
         <v>262</v>
       </c>
+      <c r="H290">
+        <v>18</v>
+      </c>
     </row>
     <row r="291" spans="1:8">
       <c r="A291" t="s">
@@ -8349,6 +8486,9 @@
       <c r="G296">
         <v>809</v>
       </c>
+      <c r="H296">
+        <v>71</v>
+      </c>
     </row>
     <row r="297" spans="1:8">
       <c r="A297" t="s">
@@ -8502,6 +8642,9 @@
       <c r="G302">
         <v>606</v>
       </c>
+      <c r="H302">
+        <v>46</v>
+      </c>
     </row>
     <row r="303" spans="1:8">
       <c r="A303" t="s">
@@ -8655,6 +8798,9 @@
       <c r="G308">
         <v>510</v>
       </c>
+      <c r="H308">
+        <v>23</v>
+      </c>
     </row>
     <row r="309" spans="1:8">
       <c r="A309" t="s">
@@ -8808,6 +8954,9 @@
       <c r="G314">
         <v>787</v>
       </c>
+      <c r="H314">
+        <v>108</v>
+      </c>
     </row>
     <row r="315" spans="1:8">
       <c r="A315" t="s">
@@ -8961,6 +9110,9 @@
       <c r="G320">
         <v>8213</v>
       </c>
+      <c r="H320">
+        <v>655</v>
+      </c>
     </row>
     <row r="321" spans="1:8">
       <c r="A321" t="s">
@@ -9114,6 +9266,9 @@
       <c r="G326">
         <v>1206</v>
       </c>
+      <c r="H326">
+        <v>77</v>
+      </c>
     </row>
     <row r="327" spans="1:8">
       <c r="A327" t="s">
@@ -9267,6 +9422,9 @@
       <c r="G332">
         <v>485</v>
       </c>
+      <c r="H332">
+        <v>44</v>
+      </c>
     </row>
     <row r="333" spans="1:8">
       <c r="A333" t="s">
@@ -9420,6 +9578,9 @@
       <c r="G338">
         <v>373</v>
       </c>
+      <c r="H338">
+        <v>23</v>
+      </c>
     </row>
     <row r="339" spans="1:8">
       <c r="A339" t="s">
@@ -9521,7 +9682,7 @@
       <c r="G342">
         <v>249</v>
       </c>
-      <c r="H342" s="2">
+      <c r="H342" s="1">
         <v>41</v>
       </c>
     </row>
@@ -9573,6 +9734,9 @@
       <c r="G344">
         <v>280</v>
       </c>
+      <c r="H344">
+        <v>26</v>
+      </c>
     </row>
     <row r="345" spans="1:8">
       <c r="A345" t="s">
@@ -9726,6 +9890,9 @@
       <c r="G350">
         <v>1462</v>
       </c>
+      <c r="H350">
+        <v>101</v>
+      </c>
     </row>
     <row r="351" spans="1:8">
       <c r="A351" t="s">
@@ -9879,6 +10046,9 @@
       <c r="G356">
         <v>336</v>
       </c>
+      <c r="H356">
+        <v>30</v>
+      </c>
     </row>
     <row r="357" spans="1:8">
       <c r="A357" t="s">
@@ -10032,6 +10202,9 @@
       <c r="G362">
         <v>3139</v>
       </c>
+      <c r="H362">
+        <v>283</v>
+      </c>
     </row>
     <row r="363" spans="1:8">
       <c r="A363" t="s">
@@ -10185,6 +10358,9 @@
       <c r="G368">
         <v>450</v>
       </c>
+      <c r="H368">
+        <v>40</v>
+      </c>
     </row>
     <row r="369" spans="1:8">
       <c r="A369" t="s">
@@ -10338,6 +10514,9 @@
       <c r="G374">
         <v>680</v>
       </c>
+      <c r="H374">
+        <v>58</v>
+      </c>
     </row>
     <row r="375" spans="1:8">
       <c r="A375" t="s">
@@ -10491,6 +10670,9 @@
       <c r="G380">
         <v>543</v>
       </c>
+      <c r="H380">
+        <v>36</v>
+      </c>
     </row>
     <row r="381" spans="1:8">
       <c r="A381" t="s">
@@ -10644,6 +10826,9 @@
       <c r="G386">
         <v>531</v>
       </c>
+      <c r="H386">
+        <v>18</v>
+      </c>
     </row>
     <row r="387" spans="1:8">
       <c r="A387" t="s">
@@ -10797,6 +10982,9 @@
       <c r="G392">
         <v>514</v>
       </c>
+      <c r="H392">
+        <v>41</v>
+      </c>
     </row>
     <row r="393" spans="1:8">
       <c r="A393" t="s">
@@ -10950,6 +11138,9 @@
       <c r="G398">
         <v>1171</v>
       </c>
+      <c r="H398">
+        <v>72</v>
+      </c>
     </row>
     <row r="399" spans="1:8">
       <c r="A399" t="s">
@@ -11103,6 +11294,9 @@
       <c r="G404">
         <v>1357</v>
       </c>
+      <c r="H404">
+        <v>81</v>
+      </c>
     </row>
     <row r="405" spans="1:8">
       <c r="A405" t="s">
@@ -11256,6 +11450,9 @@
       <c r="G410">
         <v>851</v>
       </c>
+      <c r="H410">
+        <v>68</v>
+      </c>
     </row>
     <row r="411" spans="1:8">
       <c r="A411" t="s">
@@ -11409,6 +11606,9 @@
       <c r="G416">
         <v>2820</v>
       </c>
+      <c r="H416">
+        <v>288</v>
+      </c>
     </row>
     <row r="417" spans="1:8">
       <c r="A417" t="s">
@@ -11562,6 +11762,9 @@
       <c r="G422">
         <v>869</v>
       </c>
+      <c r="H422">
+        <v>70</v>
+      </c>
     </row>
     <row r="423" spans="1:8">
       <c r="A423" t="s">
@@ -11715,6 +11918,9 @@
       <c r="G428">
         <v>933</v>
       </c>
+      <c r="H428">
+        <v>67</v>
+      </c>
     </row>
     <row r="429" spans="1:8">
       <c r="A429" t="s">
@@ -11868,6 +12074,9 @@
       <c r="G434">
         <v>1103</v>
       </c>
+      <c r="H434">
+        <v>117</v>
+      </c>
     </row>
     <row r="435" spans="1:8">
       <c r="A435" t="s">
@@ -12021,6 +12230,9 @@
       <c r="G440">
         <v>12336</v>
       </c>
+      <c r="H440">
+        <v>860</v>
+      </c>
     </row>
     <row r="441" spans="1:8">
       <c r="A441" t="s">
@@ -12174,6 +12386,9 @@
       <c r="G446">
         <v>1292</v>
       </c>
+      <c r="H446">
+        <v>172</v>
+      </c>
     </row>
     <row r="447" spans="1:8">
       <c r="A447" t="s">
@@ -12327,6 +12542,9 @@
       <c r="G452">
         <v>221</v>
       </c>
+      <c r="H452">
+        <v>22</v>
+      </c>
     </row>
     <row r="453" spans="1:8">
       <c r="A453" s="1" t="s">
@@ -12480,6 +12698,9 @@
       <c r="G458">
         <v>318</v>
       </c>
+      <c r="H458">
+        <v>13</v>
+      </c>
     </row>
     <row r="459" spans="1:8">
       <c r="A459" s="1" t="s">
@@ -12633,6 +12854,9 @@
       <c r="G464">
         <v>2875</v>
       </c>
+      <c r="H464">
+        <v>304</v>
+      </c>
     </row>
     <row r="465" spans="1:8">
       <c r="A465" t="s">
@@ -12786,6 +13010,9 @@
       <c r="G470">
         <v>734</v>
       </c>
+      <c r="H470">
+        <v>85</v>
+      </c>
     </row>
     <row r="471" spans="1:8">
       <c r="A471" t="s">
@@ -12939,6 +13166,9 @@
       <c r="G476">
         <v>2434</v>
       </c>
+      <c r="H476">
+        <v>438</v>
+      </c>
     </row>
     <row r="477" spans="1:8">
       <c r="A477" t="s">
@@ -13092,6 +13322,9 @@
       <c r="G482">
         <v>1119</v>
       </c>
+      <c r="H482">
+        <v>170</v>
+      </c>
     </row>
     <row r="483" spans="1:8">
       <c r="A483" t="s">
@@ -13245,6 +13478,9 @@
       <c r="G488">
         <v>833</v>
       </c>
+      <c r="H488">
+        <v>91</v>
+      </c>
     </row>
     <row r="489" spans="1:8">
       <c r="A489" t="s">
@@ -13398,6 +13634,9 @@
       <c r="G494">
         <v>1468</v>
       </c>
+      <c r="H494">
+        <v>150</v>
+      </c>
     </row>
     <row r="495" spans="1:8">
       <c r="A495" t="s">
@@ -13551,6 +13790,9 @@
       <c r="G500">
         <v>1478</v>
       </c>
+      <c r="H500">
+        <v>170</v>
+      </c>
     </row>
     <row r="501" spans="1:8">
       <c r="A501" t="s">
@@ -13704,6 +13946,9 @@
       <c r="G506">
         <v>733</v>
       </c>
+      <c r="H506">
+        <v>83</v>
+      </c>
     </row>
     <row r="507" spans="1:8">
       <c r="A507" t="s">
@@ -13857,6 +14102,9 @@
       <c r="G512">
         <v>4076</v>
       </c>
+      <c r="H512">
+        <v>321</v>
+      </c>
     </row>
     <row r="513" spans="1:8">
       <c r="A513" t="s">
@@ -14010,6 +14258,9 @@
       <c r="G518">
         <v>3882</v>
       </c>
+      <c r="H518">
+        <v>380</v>
+      </c>
     </row>
     <row r="519" spans="1:8">
       <c r="A519" t="s">
@@ -14163,6 +14414,9 @@
       <c r="G524">
         <v>305</v>
       </c>
+      <c r="H524">
+        <v>20</v>
+      </c>
     </row>
     <row r="525" spans="1:8">
       <c r="A525" t="s">
@@ -14316,6 +14570,9 @@
       <c r="G530">
         <v>416</v>
       </c>
+      <c r="H530">
+        <v>21</v>
+      </c>
     </row>
     <row r="531" spans="1:8">
       <c r="A531" t="s">
@@ -14469,6 +14726,9 @@
       <c r="G536">
         <v>1406</v>
       </c>
+      <c r="H536">
+        <v>229</v>
+      </c>
     </row>
     <row r="537" spans="1:8">
       <c r="A537" t="s">
@@ -14622,6 +14882,9 @@
       <c r="G542">
         <v>1351</v>
       </c>
+      <c r="H542">
+        <v>294</v>
+      </c>
     </row>
     <row r="543" spans="1:8">
       <c r="A543" t="s">
@@ -14775,6 +15038,9 @@
       <c r="G548">
         <v>2241</v>
       </c>
+      <c r="H548">
+        <v>279</v>
+      </c>
     </row>
     <row r="549" spans="1:8">
       <c r="A549" t="s">
@@ -14928,6 +15194,9 @@
       <c r="G554">
         <v>693</v>
       </c>
+      <c r="H554">
+        <v>21</v>
+      </c>
     </row>
     <row r="555" spans="1:8">
       <c r="A555" t="s">
@@ -15081,6 +15350,9 @@
       <c r="G560">
         <v>1329</v>
       </c>
+      <c r="H560">
+        <v>250</v>
+      </c>
     </row>
     <row r="561" spans="1:8">
       <c r="A561" t="s">
@@ -15234,6 +15506,9 @@
       <c r="G566">
         <v>1291</v>
       </c>
+      <c r="H566">
+        <v>155</v>
+      </c>
     </row>
     <row r="567" spans="1:8">
       <c r="A567" t="s">
@@ -15387,9 +15662,11 @@
       <c r="G572">
         <v>2008</v>
       </c>
+      <c r="H572">
+        <v>198</v>
+      </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>